<commit_message>
v2 of flytime tool
</commit_message>
<xml_diff>
--- a/tools/DDR_flytimes.xlsx
+++ b/tools/DDR_flytimes.xlsx
@@ -452,10 +452,10 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="L19" activeCellId="0" sqref="L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.9140625" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.921875" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="29.18" customWidth="1" style="2" min="1" max="1"/>
     <col width="19.72" customWidth="1" style="2" min="2" max="2"/>
@@ -561,25 +561,25 @@
         <v>10.48</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>11.48</v>
+        <v>10.88</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>72.90000000000001</v>
+        <v>72.93000000000001</v>
       </c>
       <c r="I2" s="2" t="n">
-        <v>6.9</v>
+        <v>4.6</v>
       </c>
       <c r="J2" s="2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="K2" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L2" s="2" t="n">
-        <v>72.90000000000001</v>
+        <v>177.53</v>
       </c>
     </row>
     <row r="3" ht="13.5" customHeight="1" s="3">
@@ -602,19 +602,19 @@
         </is>
       </c>
       <c r="E3" s="2" t="n">
-        <v>10.3</v>
+        <v>10.52</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>11.3</v>
+        <v>10.92</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>71.5</v>
+        <v>73.19</v>
       </c>
       <c r="I3" s="2" t="n">
-        <v>6.9</v>
+        <v>4.6</v>
       </c>
       <c r="J3" s="2" t="n">
         <v>0</v>
@@ -623,7 +623,7 @@
         <v>0</v>
       </c>
       <c r="L3" s="2" t="n">
-        <v>71.5</v>
+        <v>77.78999999999999</v>
       </c>
     </row>
     <row r="4" ht="13.5" customHeight="1" s="3">
@@ -646,19 +646,19 @@
         </is>
       </c>
       <c r="E4" s="2" t="n">
-        <v>16.42</v>
+        <v>16.7</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>17.42</v>
+        <v>17.1</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>115</v>
+        <v>116.96</v>
       </c>
       <c r="I4" s="2" t="n">
-        <v>6.9</v>
+        <v>4.6</v>
       </c>
       <c r="J4" s="2" t="n">
         <v>0</v>
@@ -667,7 +667,7 @@
         <v>0</v>
       </c>
       <c r="L4" s="2" t="n">
-        <v>115</v>
+        <v>121.56</v>
       </c>
     </row>
     <row r="5" ht="13.5" customHeight="1" s="3">
@@ -690,19 +690,19 @@
         </is>
       </c>
       <c r="E5" s="2" t="n">
-        <v>17.63</v>
+        <v>18.18</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>18.63</v>
+        <v>18.58</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>123.5</v>
+        <v>127.51</v>
       </c>
       <c r="I5" s="2" t="n">
-        <v>6.9</v>
+        <v>4.6</v>
       </c>
       <c r="J5" s="2" t="n">
         <v>0</v>
@@ -711,7 +711,7 @@
         <v>0</v>
       </c>
       <c r="L5" s="2" t="n">
-        <v>123.5</v>
+        <v>132.11</v>
       </c>
     </row>
     <row r="6" ht="13.5" customHeight="1" s="3">
@@ -734,19 +734,19 @@
         </is>
       </c>
       <c r="E6" s="2" t="n">
-        <v>17.33</v>
+        <v>17.51</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>18.33</v>
+        <v>17.91</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>121.4</v>
+        <v>122.65</v>
       </c>
       <c r="I6" s="2" t="n">
-        <v>6.9</v>
+        <v>4.6</v>
       </c>
       <c r="J6" s="2" t="n">
         <v>0</v>
@@ -755,7 +755,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="2" t="n">
-        <v>121.4</v>
+        <v>127.25</v>
       </c>
     </row>
     <row r="7" ht="13.5" customHeight="1" s="3">
@@ -778,19 +778,19 @@
         </is>
       </c>
       <c r="E7" s="2" t="n">
-        <v>17.89</v>
+        <v>17.94</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>18.89</v>
+        <v>18.34</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>125.4</v>
+        <v>125.82</v>
       </c>
       <c r="I7" s="2" t="n">
-        <v>6.9</v>
+        <v>4.6</v>
       </c>
       <c r="J7" s="2" t="n">
         <v>0</v>
@@ -799,7 +799,7 @@
         <v>0</v>
       </c>
       <c r="L7" s="2" t="n">
-        <v>125.4</v>
+        <v>130.42</v>
       </c>
     </row>
     <row r="8" ht="13.5" customHeight="1" s="3"/>
@@ -867,13 +867,13 @@
       <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.9140625" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.921875" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="29.18" customWidth="1" style="2" min="1" max="1"/>
     <col width="19.72" customWidth="1" style="2" min="2" max="2"/>
     <col width="14.03" customWidth="1" style="2" min="4" max="4"/>
     <col width="15.14" customWidth="1" style="2" min="5" max="5"/>
-    <col width="11.66" customWidth="1" style="2" min="6" max="6"/>
+    <col width="11.65" customWidth="1" style="2" min="6" max="6"/>
     <col width="13.19" customWidth="1" style="2" min="7" max="7"/>
     <col width="12.22" customWidth="1" style="2" min="8" max="8"/>
     <col width="14.86" customWidth="1" style="2" min="9" max="9"/>
@@ -973,16 +973,16 @@
         <v>11</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>12</v>
+        <v>11.4</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>76.59999999999999</v>
+        <v>76.59</v>
       </c>
       <c r="I2" s="2" t="n">
-        <v>6.9</v>
+        <v>4.6</v>
       </c>
       <c r="J2" s="2" t="n">
         <v>0</v>
@@ -991,7 +991,7 @@
         <v>0</v>
       </c>
       <c r="L2" s="2" t="n">
-        <v>76.59999999999999</v>
+        <v>81.19</v>
       </c>
     </row>
     <row r="3" ht="13.5" customHeight="1" s="3">
@@ -1017,16 +1017,16 @@
         <v>11.19</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>12.19</v>
+        <v>11.59</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>77.90000000000001</v>
+        <v>77.94</v>
       </c>
       <c r="I3" s="2" t="n">
-        <v>6.9</v>
+        <v>4.6</v>
       </c>
       <c r="J3" s="2" t="n">
         <v>0</v>
@@ -1035,7 +1035,7 @@
         <v>0</v>
       </c>
       <c r="L3" s="2" t="n">
-        <v>77.90000000000001</v>
+        <v>82.53999999999999</v>
       </c>
     </row>
     <row r="4" ht="13.5" customHeight="1" s="3">
@@ -1058,19 +1058,19 @@
         </is>
       </c>
       <c r="E4" s="2" t="n">
-        <v>16.44</v>
+        <v>18.18</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>17.44</v>
+        <v>18.58</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>115.1</v>
+        <v>127.41</v>
       </c>
       <c r="I4" s="2" t="n">
-        <v>6.9</v>
+        <v>4.6</v>
       </c>
       <c r="J4" s="2" t="n">
         <v>0</v>
@@ -1079,7 +1079,7 @@
         <v>0</v>
       </c>
       <c r="L4" s="2" t="n">
-        <v>115.1</v>
+        <v>132.01</v>
       </c>
     </row>
     <row r="5" ht="13.5" customHeight="1" s="3">
@@ -1102,19 +1102,19 @@
         </is>
       </c>
       <c r="E5" s="2" t="n">
-        <v>16.98</v>
+        <v>17.62</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>17.98</v>
+        <v>18.02</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>118.9</v>
+        <v>123.45</v>
       </c>
       <c r="I5" s="2" t="n">
-        <v>6.9</v>
+        <v>4.6</v>
       </c>
       <c r="J5" s="2" t="n">
         <v>0</v>
@@ -1123,7 +1123,7 @@
         <v>0</v>
       </c>
       <c r="L5" s="2" t="n">
-        <v>118.9</v>
+        <v>128.05</v>
       </c>
     </row>
     <row r="6" ht="13.5" customHeight="1" s="3">
@@ -1146,19 +1146,19 @@
         </is>
       </c>
       <c r="E6" s="2" t="n">
-        <v>18.51</v>
+        <v>19.19</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>19.51</v>
+        <v>19.59</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>129.8</v>
+        <v>134.58</v>
       </c>
       <c r="I6" s="2" t="n">
-        <v>6.9</v>
+        <v>4.6</v>
       </c>
       <c r="J6" s="2" t="n">
         <v>0</v>
@@ -1167,7 +1167,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="2" t="n">
-        <v>129.8</v>
+        <v>139.18</v>
       </c>
     </row>
     <row r="7" ht="13.5" customHeight="1" s="3">
@@ -1190,19 +1190,19 @@
         </is>
       </c>
       <c r="E7" s="2" t="n">
-        <v>19.19</v>
+        <v>21.2</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>20.19</v>
+        <v>21.6</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>134.6</v>
+        <v>148.16</v>
       </c>
       <c r="I7" s="2" t="n">
-        <v>6.9</v>
+        <v>4.6</v>
       </c>
       <c r="J7" s="2" t="n">
         <v>0</v>
@@ -1211,7 +1211,7 @@
         <v>0</v>
       </c>
       <c r="L7" s="2" t="n">
-        <v>134.6</v>
+        <v>152.76</v>
       </c>
     </row>
     <row r="8" ht="13.5" customHeight="1" s="3">

</xml_diff>